<commit_message>
can submit question and search question on UI
</commit_message>
<xml_diff>
--- a/project/Tag_Database.xlsx
+++ b/project/Tag_Database.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,79 +556,93 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>ทำการบ้านเลขไม่ได้เลยทำยังไงดี</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>o</t>
+          <t>ทำการบ้าน</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>การเรียน</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>v</t>
+          <t>เลข</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>w</t>
+          <t>คณิตศาสตร์</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>q</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>t</t>
+          <t>การบ้าน</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>คณิตศาสตร์ยากจัง</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>คณิตศาสตร์</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>u</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>w</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>z</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>f</t>
+          <t>การบ้าน</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ทำไมการเรียนออนไลน์ถึงมีการบ้านเยอะจัง</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>การเรียน</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>การบ้าน</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ผมเกลียดเลข แต่แม่บังคับให้เรียนพิเศษเพิ่ม ทำอย่างไรดี</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>เลข</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>คณิตศาสตร์</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>แม่</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ครอบครัว</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clear/submit delete all manual tag
</commit_message>
<xml_diff>
--- a/project/Tag_Database.xlsx
+++ b/project/Tag_Database.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +646,99 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>สูตรเรขาคณิตจำยากจัง</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>เรขาคณิต</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>คณิตศาสตร์</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ลูกแมวสามารถให้อาหารอะไรได้บ้าง</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>แมว</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>สัตว์เลี้ยง</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>สัตว์</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ทำอย่างไรแมวถึงจะยอมอาบน้ำ</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>แมว</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>สัตว์เลี้ยง</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>สัตว์</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>อาบน้ำแมว</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>เผลอซักผ้าสีปนกับผ้าขาว ทำอย่างไรดี</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ซักผ้า</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>งานบ้าน</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ผ้าสี</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ผ้าขาว</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more question and word dict
</commit_message>
<xml_diff>
--- a/project/Tag_Database.xlsx
+++ b/project/Tag_Database.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,6 +739,121 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ทำไมสินค้ายี่ห้อ "Apple" ถึงราคาแพง</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>สินค้า</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ของแพง</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ท้องเสียมา 2 วันติดแล้ว กินยาตัวไหนดี</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ท้องเสีย</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>เจ็บป่วย</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ยา</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>เครื่องซักผ้าเสีย ซักผ้าอยู่ดี ๆ ก็ดับไปเลย</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>เครื่องซักผ้า</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>เครื่องใช้ไฟฟ้า</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ซักผ้า</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>งานบ้าน</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>แม่ผัวน่ารำคาญมาก หาเรื่องบ่นเราได้ตลอดเลย ทำยังไงได้บ้างคะ</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>แม่ผัว</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ครอบครัว</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ปัญหาครอบครัว</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>กลิ่นเต่าแฟนเหม็นมาก รับไม่ได้เลย สามารถทำยังไงได้บ้าง</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>กลิ่นเต่า</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ร่างกาย</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>กลิ่นรักแร้</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
in input box text
</commit_message>
<xml_diff>
--- a/project/Tag_Database.xlsx
+++ b/project/Tag_Database.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1107,6 +1107,52 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ปั่นงานไม่ทันแล้วทำอย่างไรดี</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>งาน</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>เวลาชีวิต</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>งานเยอะมากเลย เลือกทำไม่ถูก</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>งาน</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>วิธีการเลี้ยงปลาทอง</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ปลาทอง</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>สัตว์เลี้ยง</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>